<commit_message>
Aggiornamento menu.xlsx via backend
</commit_message>
<xml_diff>
--- a/menu.xlsx
+++ b/menu.xlsx
@@ -5,22 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48077\Desktop\Appoggio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10677\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C687F69-2566-418C-8B55-18FEBFE18E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D620915-A7EA-45FD-8C4C-BFB41E935D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" activeTab="1" xr2:uid="{B82D7E25-2410-48DD-822B-69CDB00A7CF6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{F4F67787-3229-48A4-A7FF-03855324C210}"/>
   </bookViews>
   <sheets>
     <sheet name="MENU ESTATE 2025" sheetId="1" r:id="rId1"/>
     <sheet name="MENU CELIACI" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Excel_BuiltIn_Print_Area" localSheetId="0">'MENU ESTATE 2025'!$A$1:$F$40</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'MENU ESTATE 2025'!$A$1:$F$39</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area" localSheetId="0">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="178">
-  <si>
-    <t>MENU LEONARDO CASCINA COSTA  2025 – ESTATE    DAL 23/06/25</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="179">
   <si>
     <r>
       <rPr>
@@ -170,13 +166,7 @@
     <t>INSALATATA DI PASTA AI CARCIOFI E OLIVE</t>
   </si>
   <si>
-    <t>PASTA AL PESTO</t>
-  </si>
-  <si>
     <t>PASTA AL GAZPACHO</t>
-  </si>
-  <si>
-    <t>PASTA ALLE COZZE</t>
   </si>
   <si>
     <t>ZUPPA DI PORRI</t>
@@ -624,6 +614,18 @@
   </si>
   <si>
     <t xml:space="preserve">TACCHINO FUME' CON RUCOLA </t>
+  </si>
+  <si>
+    <t>GNOCCHI AL PESTO</t>
+  </si>
+  <si>
+    <t>PASTA AL SALMONE</t>
+  </si>
+  <si>
+    <t>BRACIOLA DI MAIALE ALBURRO</t>
+  </si>
+  <si>
+    <t>MENU LEONARDO CASCINA COSTA  2025 – ESTATE    DAL 01/09/25</t>
   </si>
 </sst>
 </file>
@@ -722,7 +724,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -731,14 +733,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="53"/>
-        <bgColor indexed="52"/>
+        <fgColor indexed="40"/>
+        <bgColor indexed="49"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="40"/>
-        <bgColor indexed="49"/>
+        <fgColor indexed="9"/>
+        <bgColor indexed="26"/>
       </patternFill>
     </fill>
     <fill>
@@ -749,7 +751,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor indexed="53"/>
+        <bgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="26"/>
       </patternFill>
     </fill>
@@ -763,10 +771,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="8"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="medium">
@@ -779,7 +787,7 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="8"/>
       </right>
       <top style="medium">
@@ -792,34 +800,6 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
@@ -982,11 +962,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -997,64 +1005,64 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1078,21 +1086,30 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1192,10 +1209,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Immagine 1">
+        <xdr:cNvPr id="1030" name="Immagine 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A00314A9-549A-55C4-D1D3-15C7E689064D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DBF9E32-0F2E-7E78-354F-52E14C05A6F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1242,7 +1259,7 @@
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525" cap="flat">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="3465A4"/>
               </a:solidFill>
@@ -1285,10 +1302,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2049" name="Immagine 1">
+        <xdr:cNvPr id="2054" name="Immagine 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1718C42E-F098-D26A-7142-46CC710BD42A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5429E40E-D776-7751-64B1-4645F5596C0F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1335,7 +1352,7 @@
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525" cap="flat">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="3465A4"/>
               </a:solidFill>
@@ -1362,7 +1379,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1674,17 +1691,6 @@
           <a:tailEnd type="none" w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
       </a:spPr>
       <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
       <a:lstStyle/>
@@ -1716,37 +1722,21 @@
           <a:tailEnd type="none" w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
       </a:spPr>
       <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
       <a:lstStyle/>
     </a:lnDef>
   </a:objectDefaults>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E4EDDA-CB86-4210-A448-9B4FD7ACC6A4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF44A27-A3E9-4234-8525-EAFE54395042}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -1759,14 +1749,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="A1" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1777,599 +1767,599 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="B5" s="34"/>
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="6" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="12" t="s">
+    </row>
+    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="E8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="F8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="9" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="E9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="F9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="9" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="E10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="F10" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="14" t="s">
+    </row>
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="16" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="16" t="s">
+      <c r="D11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="F11" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="B12" s="37"/>
+      <c r="C12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="21" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="14" t="s">
+    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="34"/>
+      <c r="C19" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="34"/>
+      <c r="C26" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="25"/>
+    </row>
+    <row r="27" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G27" s="25"/>
+    </row>
+    <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="25"/>
+    </row>
+    <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G29" s="25"/>
+    </row>
+    <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G30" s="25"/>
+    </row>
+    <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" s="25"/>
+    </row>
+    <row r="32" spans="1:7" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G32" s="25"/>
+    </row>
+    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" s="34"/>
+      <c r="C33" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="34"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="G26" s="25"/>
-    </row>
-    <row r="27" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="G27" s="25"/>
-    </row>
-    <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="33"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G28" s="25"/>
-    </row>
-    <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="33"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="G29" s="25"/>
-    </row>
-    <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G30" s="25"/>
-    </row>
-    <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="33"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="G31" s="25"/>
-    </row>
-    <row r="32" spans="1:7" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="33"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="G32" s="25"/>
-    </row>
-    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="33"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="33"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="33"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F36" s="23" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="33"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="33"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D38" s="13" t="s">
+      <c r="D39" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E39" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F39" s="18" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="33"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -2405,10 +2395,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D677FE29-4988-45E8-B412-07F8BA84A151}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB22AC35-865D-45CB-BFB6-6FDD2F9E51E6}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -2422,527 +2412,527 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+    </row>
+    <row r="3" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-    </row>
-    <row r="3" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="E4" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D4" s="6" t="s">
+    </row>
+    <row r="5" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="D5" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="E5" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="9" t="s">
+    <row r="6" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E6" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="F5" s="13" t="s">
+    </row>
+    <row r="7" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="9" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="9" t="s">
+      <c r="D7" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E8" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="13" t="s">
+      <c r="F9" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="21" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="16" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="6" t="s">
+      <c r="D15" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="34"/>
+      <c r="C16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="24" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="25"/>
+    </row>
+    <row r="21" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" s="25"/>
+    </row>
+    <row r="22" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="34"/>
+      <c r="C22" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G22" s="25"/>
+    </row>
+    <row r="23" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E23" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="G23" s="25"/>
+    </row>
+    <row r="24" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="9" t="s">
+      <c r="D24" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G24" s="25"/>
+    </row>
+    <row r="25" spans="1:7" s="26" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="G25" s="25"/>
+    </row>
+    <row r="26" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="34"/>
+      <c r="C28" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E11" s="9" t="s">
+      <c r="E30" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F30" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="F11" s="13" t="s">
+    </row>
+    <row r="31" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="9" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="21" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E17" s="9" t="s">
+      <c r="D31" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="24" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" s="25"/>
-    </row>
-    <row r="21" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="G21" s="25"/>
-    </row>
-    <row r="22" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="G22" s="25"/>
-    </row>
-    <row r="23" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="F23" s="13" t="s">
+      <c r="E31" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="G23" s="25"/>
-    </row>
-    <row r="24" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="G24" s="25"/>
-    </row>
-    <row r="25" spans="1:7" s="26" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="G25" s="25"/>
-    </row>
-    <row r="26" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="33"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="F31" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="33"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="33"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="33"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="33" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="33"/>
-      <c r="B33" s="33"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
       <c r="C33" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>